<commit_message>
Update payroll output format and add gross pay calculation
</commit_message>
<xml_diff>
--- a/Outputs/Payslips/Alice Murphy.xlsx
+++ b/Outputs/Payslips/Alice Murphy.xlsx
@@ -3,22 +3,23 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="3090" yWindow="1215" windowWidth="21600" windowHeight="11295" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Payslip" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="162913" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="16">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -29,13 +30,6 @@
     <font>
       <name val="Arial"/>
       <family val="2"/>
-      <b val="1"/>
-      <color rgb="FF3573A7"/>
-      <sz val="24"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="2"/>
       <sz val="24"/>
     </font>
     <font>
@@ -43,13 +37,6 @@
       <family val="2"/>
       <b val="1"/>
       <sz val="24"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="2"/>
-      <b val="1"/>
-      <color rgb="FF3573A7"/>
-      <sz val="28"/>
     </font>
     <font>
       <name val="Arial"/>
@@ -105,8 +92,35 @@
       <color rgb="FF000000"/>
       <sz val="11"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <b val="1"/>
+      <color theme="9"/>
+      <sz val="24"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <b val="1"/>
+      <color theme="9"/>
+      <sz val="28"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <color theme="9" tint="0.3999755851924192"/>
+      <sz val="9"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill/>
     </fill>
@@ -115,31 +129,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF7BACD5"/>
+        <fgColor theme="9"/>
         <bgColor rgb="FF6FA8DC"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD2E2F0"/>
+        <fgColor theme="9" tint="0.3999755851924192"/>
         <bgColor rgb="FFF3F3F3"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor rgb="FFF3F3F3"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
+        <fgColor theme="9" tint="0.3999755851924192"/>
         <bgColor rgb="FFD9D9D9"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
+        <fgColor theme="9" tint="0.3999755851924192"/>
         <bgColor rgb="FF999999"/>
       </patternFill>
     </fill>
@@ -204,137 +212,142 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="14" fontId="8" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="10" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="5" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="165" fontId="7" fillId="5" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="6" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="5" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="6" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="5" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -677,8 +690,8 @@
   </sheetPr>
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -690,238 +703,214 @@
   </cols>
   <sheetData>
     <row r="1" ht="35.25" customHeight="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Financial IT Solutions Ltd</t>
-        </is>
-      </c>
-      <c r="B1" s="2" t="n"/>
-      <c r="C1" s="3" t="n"/>
-      <c r="D1" s="4" t="inlineStr">
+      <c r="A1" s="20" t="inlineStr">
+        <is>
+          <t>Luke Maycock Portraiture Ltd.</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="n"/>
+      <c r="C1" s="2" t="n"/>
+      <c r="D1" s="21" t="inlineStr">
         <is>
           <t>PAYSLIP</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="inlineStr">
+      <c r="A2" s="26" t="inlineStr">
         <is>
           <t>Somewhere in Ireland</t>
         </is>
       </c>
-      <c r="B2" s="6" t="n"/>
-      <c r="C2" s="7" t="n"/>
-      <c r="D2" s="7" t="n"/>
+      <c r="B2" s="3" t="n"/>
+      <c r="C2" s="4" t="n"/>
+      <c r="D2" s="4" t="n"/>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="inlineStr">
+      <c r="A3" s="26" t="inlineStr">
         <is>
           <t>Phone: +353 00 0000 0000</t>
         </is>
       </c>
-      <c r="B3" s="6" t="n"/>
-      <c r="C3" s="7" t="n"/>
-      <c r="D3" s="7" t="n"/>
+      <c r="B3" s="3" t="n"/>
+      <c r="C3" s="4" t="n"/>
+      <c r="D3" s="4" t="n"/>
     </row>
     <row r="4">
-      <c r="A4" s="8" t="n"/>
-      <c r="B4" s="9" t="n"/>
-      <c r="C4" s="10" t="n"/>
-      <c r="D4" s="10" t="n"/>
+      <c r="A4" s="5" t="n"/>
+      <c r="B4" s="6" t="n"/>
+      <c r="C4" s="7" t="n"/>
+      <c r="D4" s="7" t="n"/>
     </row>
     <row r="5">
-      <c r="A5" s="11" t="inlineStr">
+      <c r="A5" s="22" t="inlineStr">
         <is>
           <t>EMPLOYEE INFORMATION</t>
         </is>
       </c>
-      <c r="B5" s="9" t="n"/>
-      <c r="C5" s="12" t="inlineStr">
+      <c r="B5" s="6" t="n"/>
+      <c r="C5" s="23" t="inlineStr">
         <is>
           <t>PAY DATE</t>
         </is>
       </c>
-      <c r="D5" s="13" t="inlineStr">
+      <c r="D5" s="24" t="inlineStr">
         <is>
           <t>PAY TYPE</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="14" t="inlineStr">
+      <c r="A6" s="8" t="inlineStr">
         <is>
           <t>Alice Murphy</t>
         </is>
       </c>
-      <c r="B6" s="9" t="n"/>
-      <c r="C6" s="15" t="inlineStr">
-        <is>
-          <t>&lt;current date&gt;</t>
-        </is>
-      </c>
-      <c r="D6" s="16" t="inlineStr">
+      <c r="B6" s="6" t="n"/>
+      <c r="C6" s="25" t="inlineStr">
+        <is>
+          <t>29/01/2026</t>
+        </is>
+      </c>
+      <c r="D6" s="38" t="inlineStr">
         <is>
           <t>Weekly</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="17" t="inlineStr">
-        <is>
-          <t>123 Any Court Road</t>
-        </is>
-      </c>
-      <c r="B7" s="18" t="inlineStr">
+      <c r="A7" s="9" t="inlineStr">
+        <is>
+          <t>Address 1</t>
+        </is>
+      </c>
+      <c r="B7" s="10" t="inlineStr">
         <is>
           <t>[42]</t>
         </is>
       </c>
-      <c r="C7" s="12" t="inlineStr">
-        <is>
-          <t>PAYROLL #</t>
-        </is>
-      </c>
-      <c r="D7" s="13" t="inlineStr">
+      <c r="C7" s="6" t="n"/>
+      <c r="D7" s="24" t="inlineStr">
         <is>
           <t>PPS NUMBER</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="17" t="inlineStr">
-        <is>
-          <t>Dublin, Ireland</t>
-        </is>
-      </c>
-      <c r="B8" s="9" t="n"/>
-      <c r="C8" s="19" t="inlineStr">
-        <is>
-          <t>&lt;payroll number&gt;</t>
-        </is>
-      </c>
-      <c r="D8" s="20" t="inlineStr">
-        <is>
-          <t>&lt;PPSN&gt;</t>
+      <c r="A8" s="9" t="inlineStr">
+        <is>
+          <t>Address 2</t>
+        </is>
+      </c>
+      <c r="B8" s="6" t="n"/>
+      <c r="C8" s="6" t="n"/>
+      <c r="D8" s="39" t="inlineStr">
+        <is>
+          <t>1234567A</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="17" t="inlineStr">
+      <c r="A9" s="9" t="inlineStr">
         <is>
           <t>Phone: +353 00 0000 0000</t>
         </is>
       </c>
-      <c r="B9" s="9" t="n"/>
-      <c r="C9" s="21" t="n"/>
-      <c r="D9" s="21" t="n"/>
+      <c r="B9" s="6" t="n"/>
+      <c r="C9" s="11" t="n"/>
+      <c r="D9" s="11" t="n"/>
     </row>
     <row r="10">
-      <c r="A10" s="17" t="inlineStr">
+      <c r="A10" s="9" t="inlineStr">
         <is>
           <t>Email: name@provider.com</t>
         </is>
       </c>
-      <c r="B10" s="9" t="n"/>
-      <c r="C10" s="21" t="inlineStr">
+      <c r="B10" s="6" t="n"/>
+      <c r="C10" s="11" t="inlineStr">
         <is>
           <t>Payment Method:</t>
         </is>
       </c>
-      <c r="D10" s="22" t="inlineStr">
-        <is>
-          <t>Check</t>
+      <c r="D10" s="12" t="inlineStr">
+        <is>
+          <t>Electronic</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="23" t="n"/>
-      <c r="B11" s="9" t="n"/>
-      <c r="C11" s="21" t="n"/>
-      <c r="D11" s="21" t="n"/>
+      <c r="A11" s="13" t="n"/>
+      <c r="B11" s="6" t="n"/>
+      <c r="C11" s="11" t="n"/>
+      <c r="D11" s="11" t="n"/>
     </row>
     <row r="12">
-      <c r="A12" s="24" t="inlineStr">
+      <c r="A12" s="27" t="inlineStr">
         <is>
           <t>EARNINGS</t>
         </is>
       </c>
-      <c r="B12" s="25" t="inlineStr">
+      <c r="B12" s="28" t="inlineStr">
         <is>
           <t>HOURS</t>
         </is>
       </c>
-      <c r="C12" s="25" t="inlineStr">
+      <c r="C12" s="28" t="inlineStr">
         <is>
           <t>RATE</t>
         </is>
       </c>
-      <c r="D12" s="26" t="inlineStr">
+      <c r="D12" s="29" t="inlineStr">
         <is>
           <t>CURRENT</t>
         </is>
       </c>
     </row>
     <row r="13" ht="24" customHeight="1">
-      <c r="A13" s="27" t="inlineStr">
+      <c r="A13" s="14" t="inlineStr">
         <is>
           <t>Standard Pay</t>
         </is>
       </c>
-      <c r="B13" s="27" t="n">
+      <c r="B13" s="14" t="n">
         <v>35</v>
       </c>
-      <c r="C13" s="27" t="n">
+      <c r="C13" s="14" t="n">
         <v>22</v>
       </c>
-      <c r="D13" s="28" t="n">
+      <c r="D13" s="15" t="n">
         <v>770</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="27" t="inlineStr">
-        <is>
-          <t>Commission and Bonus</t>
-        </is>
-      </c>
-      <c r="B14" s="27" t="n"/>
-      <c r="C14" s="29" t="n"/>
-      <c r="D14" s="28" t="n">
+      <c r="A14" s="14" t="inlineStr">
+        <is>
+          <t>Employee Bonus</t>
+        </is>
+      </c>
+      <c r="B14" s="14" t="n"/>
+      <c r="C14" s="16" t="n"/>
+      <c r="D14" s="15" t="n">
         <v>500</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="27" t="inlineStr">
-        <is>
-          <t>Sick Pay</t>
-        </is>
-      </c>
-      <c r="B15" s="27" t="n"/>
-      <c r="C15" s="29" t="n"/>
-      <c r="D15" s="28" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="A15" s="14" t="n"/>
+      <c r="B15" s="14" t="n"/>
+      <c r="C15" s="16" t="n"/>
+      <c r="D15" s="15" t="n"/>
     </row>
     <row r="16">
-      <c r="A16" s="27" t="inlineStr">
-        <is>
-          <t>Expenses</t>
-        </is>
-      </c>
-      <c r="B16" s="27" t="n"/>
-      <c r="C16" s="29" t="n"/>
-      <c r="D16" s="28" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="A16" s="14" t="n"/>
+      <c r="B16" s="14" t="n"/>
+      <c r="C16" s="16" t="n"/>
+      <c r="D16" s="15" t="n"/>
     </row>
     <row r="17">
-      <c r="A17" s="27" t="n"/>
-      <c r="B17" s="27" t="n"/>
-      <c r="C17" s="29" t="n"/>
-      <c r="D17" s="28" t="n"/>
+      <c r="A17" s="14" t="n"/>
+      <c r="B17" s="14" t="n"/>
+      <c r="C17" s="16" t="n"/>
+      <c r="D17" s="15" t="n"/>
     </row>
     <row r="18">
       <c r="A18" s="30" t="n"/>
@@ -931,105 +920,106 @@
           <t>GROSS PAY</t>
         </is>
       </c>
-      <c r="D18" s="40" t="inlineStr">
-        <is>
-          <t>&lt;GrossPay&gt;</t>
-        </is>
+      <c r="D18" s="40" t="n">
+        <v>1370</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="23" t="n"/>
-      <c r="B19" s="9" t="n"/>
-      <c r="C19" s="9" t="n"/>
-      <c r="D19" s="34" t="n"/>
+      <c r="A19" s="13" t="n"/>
+      <c r="B19" s="6" t="n"/>
+      <c r="C19" s="6" t="n"/>
+      <c r="D19" s="17" t="n"/>
     </row>
     <row r="20">
-      <c r="A20" s="24" t="inlineStr">
+      <c r="A20" s="27" t="inlineStr">
         <is>
           <t>DEDUCTIONS</t>
         </is>
       </c>
-      <c r="B20" s="25" t="n"/>
-      <c r="C20" s="25" t="n"/>
-      <c r="D20" s="26" t="inlineStr">
+      <c r="B20" s="28" t="n"/>
+      <c r="C20" s="28" t="n"/>
+      <c r="D20" s="29" t="inlineStr">
         <is>
           <t>CURRENT</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="27" t="inlineStr">
+      <c r="A21" s="14" t="inlineStr">
         <is>
           <t>PAYE Tax</t>
         </is>
       </c>
-      <c r="B21" s="27" t="n"/>
-      <c r="C21" s="27" t="n"/>
-      <c r="D21" s="28" t="n">
+      <c r="B21" s="14" t="n"/>
+      <c r="C21" s="14" t="n"/>
+      <c r="D21" s="15" t="n">
         <v>274</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="27" t="n"/>
-      <c r="B22" s="27" t="n"/>
-      <c r="C22" s="27" t="n"/>
-      <c r="D22" s="28" t="n"/>
+      <c r="A22" s="14" t="inlineStr">
+        <is>
+          <t>Benefit In Kind</t>
+        </is>
+      </c>
+      <c r="B22" s="14" t="n"/>
+      <c r="C22" s="14" t="n"/>
+      <c r="D22" s="15" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="23">
-      <c r="A23" s="27" t="n"/>
-      <c r="B23" s="27" t="n"/>
-      <c r="C23" s="27" t="n"/>
-      <c r="D23" s="28" t="n"/>
+      <c r="A23" s="14" t="n"/>
+      <c r="B23" s="14" t="n"/>
+      <c r="C23" s="14" t="n"/>
+      <c r="D23" s="15" t="n"/>
     </row>
     <row r="24">
       <c r="A24" s="30" t="n"/>
       <c r="B24" s="31" t="n"/>
-      <c r="C24" s="35" t="inlineStr">
+      <c r="C24" s="34" t="inlineStr">
         <is>
           <t>TOTAL DEDUCTIONS</t>
         </is>
       </c>
-      <c r="D24" s="40" t="inlineStr">
-        <is>
-          <t>&lt;TotalDeductions&gt;</t>
-        </is>
+      <c r="D24" s="41">
+        <f>SUM(D21:D23)</f>
+        <v/>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A25" s="23" t="n"/>
-      <c r="B25" s="9" t="n"/>
-      <c r="C25" s="9" t="n"/>
-      <c r="D25" s="34" t="n"/>
+      <c r="A25" s="13" t="n"/>
+      <c r="B25" s="6" t="n"/>
+      <c r="C25" s="6" t="n"/>
+      <c r="D25" s="17" t="n"/>
     </row>
     <row r="26" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A26" s="23" t="n"/>
-      <c r="B26" s="9" t="n"/>
-      <c r="C26" s="36" t="inlineStr">
+      <c r="A26" s="13" t="n"/>
+      <c r="B26" s="6" t="n"/>
+      <c r="C26" s="35" t="inlineStr">
         <is>
           <t>NET PAY</t>
         </is>
       </c>
-      <c r="D26" s="41" t="inlineStr">
-        <is>
-          <t>&lt;NetPay&gt;</t>
-        </is>
+      <c r="D26" s="42" t="n">
+        <v>1096</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="23" t="n"/>
-      <c r="B27" s="9" t="n"/>
-      <c r="C27" s="9" t="n"/>
-      <c r="D27" s="9" t="n"/>
+      <c r="A27" s="13" t="n"/>
+      <c r="B27" s="6" t="n"/>
+      <c r="C27" s="6" t="n"/>
+      <c r="D27" s="6" t="n"/>
     </row>
     <row r="28">
-      <c r="A28" s="38" t="inlineStr">
+      <c r="A28" s="18" t="inlineStr">
         <is>
           <t>If you have any questions about this payslip, please contact:</t>
         </is>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="39" t="inlineStr">
+      <c r="A29" s="19" t="inlineStr">
         <is>
           <t>[Name, Phone, email@address.com]</t>
         </is>

</xml_diff>